<commit_message>
Add 2nd prototype economy
</commit_message>
<xml_diff>
--- a/AIE Year 2/Psychology and Economies/Greco Feudal Feedback.xlsx
+++ b/AIE Year 2/Psychology and Economies/Greco Feudal Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s200479\Repos\Williams_Backpack\AIE Year 2\Psychology and Economies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E35A38-A7B6-4D92-8CE8-9A922B8870CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B4631B-84C2-4EDD-BF57-07A201075CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{46E08FCF-ADDE-46E4-8514-CE4E35947774}"/>
+    <workbookView xWindow="4095" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{46E08FCF-ADDE-46E4-8514-CE4E35947774}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -69,8 +69,10 @@
     <t>Myles</t>
   </si>
   <si>
-    <t>•Identify a moral arguement
-•</t>
+    <t>•Identify a moral argument</t>
+  </si>
+  <si>
+    <t>Flesh out the theme and message I'm trying to tell with the game</t>
   </si>
 </sst>
 </file>
@@ -438,40 +440,40 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -489,7 +491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -498,6 +500,9 @@
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>